<commit_message>
Open Spreadsheet - no changes
</commit_message>
<xml_diff>
--- a/birm_res_check.xlsx
+++ b/birm_res_check.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
   </bookViews>
   <sheets>
     <sheet name="Birm_res" sheetId="1" r:id="rId1"/>
@@ -3476,7 +3476,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="13" x14ac:knownFonts="1">
     <font>
@@ -3715,13 +3715,13 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3758,7 +3758,7 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3770,9 +3770,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="4" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3789,14 +3789,14 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -3807,7 +3807,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3821,11 +3821,11 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3842,14 +3842,14 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="8" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3863,15 +3863,15 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="9" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="1" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="12" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -4186,7 +4186,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M439"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="O91" sqref="O91"/>
     </sheetView>
   </sheetViews>
@@ -33635,8 +33635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P427"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="P3" sqref="P3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -33667,6 +33667,14 @@
       <c r="H2" s="69" t="s">
         <v>29</v>
       </c>
+      <c r="I2" s="1">
+        <f>SUM($F2:F$93)</f>
+        <v>209</v>
+      </c>
+      <c r="K2">
+        <f>SUM(M2:M10)</f>
+        <v>17</v>
+      </c>
       <c r="L2" s="70">
         <v>3</v>
       </c>
@@ -33680,8 +33688,8 @@
         <v>176</v>
       </c>
       <c r="P2">
-        <f>SUM(M2:M10)</f>
-        <v>17</v>
+        <f>I5</f>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -33709,6 +33717,10 @@
       <c r="H3" s="69" t="s">
         <v>43</v>
       </c>
+      <c r="I3" s="1">
+        <f>SUM($F3:F$93)</f>
+        <v>199</v>
+      </c>
       <c r="L3" s="70">
         <v>6</v>
       </c>
@@ -33720,6 +33732,10 @@
       </c>
       <c r="O3" s="70" t="s">
         <v>178</v>
+      </c>
+      <c r="P3">
+        <f>I6</f>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -33747,6 +33763,10 @@
       <c r="H4" s="69" t="s">
         <v>32</v>
       </c>
+      <c r="I4" s="1">
+        <f>SUM($F4:F$93)</f>
+        <v>196</v>
+      </c>
       <c r="L4" s="1">
         <v>24</v>
       </c>
@@ -33758,6 +33778,10 @@
       </c>
       <c r="O4" s="1" t="s">
         <v>999</v>
+      </c>
+      <c r="P4">
+        <f>I23</f>
+        <v>116</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -33785,6 +33809,10 @@
       <c r="H5" s="69" t="s">
         <v>27</v>
       </c>
+      <c r="I5" s="1">
+        <f>SUM($F5:F$93)</f>
+        <v>190</v>
+      </c>
       <c r="L5" s="1">
         <v>55</v>
       </c>
@@ -33823,6 +33851,10 @@
       <c r="H6" s="69" t="s">
         <v>40</v>
       </c>
+      <c r="I6" s="1">
+        <f>SUM($F6:F$93)</f>
+        <v>184</v>
+      </c>
       <c r="L6" s="1">
         <v>70</v>
       </c>
@@ -33861,6 +33893,10 @@
       <c r="H7" s="69" t="s">
         <v>31</v>
       </c>
+      <c r="I7" s="1">
+        <f>SUM($F7:F$93)</f>
+        <v>183</v>
+      </c>
       <c r="L7" s="1">
         <v>72</v>
       </c>
@@ -33899,6 +33935,10 @@
       <c r="H8" s="69" t="s">
         <v>165</v>
       </c>
+      <c r="I8" s="1">
+        <f>SUM($F8:F$93)</f>
+        <v>180</v>
+      </c>
       <c r="L8" s="1">
         <v>74</v>
       </c>
@@ -33910,6 +33950,10 @@
       </c>
       <c r="O8" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="P8">
+        <f>I69</f>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -33937,6 +33981,10 @@
       <c r="H9" s="69" t="s">
         <v>45</v>
       </c>
+      <c r="I9" s="1">
+        <f>SUM($F9:F$93)</f>
+        <v>177</v>
+      </c>
       <c r="L9" s="1">
         <v>75</v>
       </c>
@@ -33975,6 +34023,10 @@
       <c r="H10" s="69" t="s">
         <v>9</v>
       </c>
+      <c r="I10" s="1">
+        <f>SUM($F10:F$93)</f>
+        <v>176</v>
+      </c>
       <c r="L10" s="1">
         <v>82</v>
       </c>
@@ -33986,6 +34038,10 @@
       </c>
       <c r="O10" s="1" t="s">
         <v>392</v>
+      </c>
+      <c r="P10">
+        <f>I76</f>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -34013,6 +34069,10 @@
       <c r="H11" s="69" t="s">
         <v>75</v>
       </c>
+      <c r="I11" s="1">
+        <f>SUM($F11:F$93)</f>
+        <v>173</v>
+      </c>
       <c r="L11" s="1">
         <v>87</v>
       </c>
@@ -34051,6 +34111,10 @@
       <c r="H12" s="69" t="s">
         <v>48</v>
       </c>
+      <c r="I12" s="1">
+        <f>SUM($F12:F$93)</f>
+        <v>170</v>
+      </c>
       <c r="L12" s="1">
         <v>90</v>
       </c>
@@ -34089,6 +34153,10 @@
       <c r="H13" s="69" t="s">
         <v>50</v>
       </c>
+      <c r="I13" s="1">
+        <f>SUM($F13:F$93)</f>
+        <v>164</v>
+      </c>
       <c r="L13" s="1">
         <v>94</v>
       </c>
@@ -34127,6 +34195,10 @@
       <c r="H14" s="69" t="s">
         <v>117</v>
       </c>
+      <c r="I14" s="1">
+        <f>SUM($F14:F$93)</f>
+        <v>163</v>
+      </c>
       <c r="L14" s="1">
         <v>97</v>
       </c>
@@ -34138,6 +34210,10 @@
       </c>
       <c r="O14" s="1" t="s">
         <v>78</v>
+      </c>
+      <c r="P14">
+        <f>I86</f>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
@@ -34165,6 +34241,10 @@
       <c r="H15" s="69" t="s">
         <v>70</v>
       </c>
+      <c r="I15" s="1">
+        <f>SUM($F15:F$93)</f>
+        <v>162</v>
+      </c>
       <c r="L15" s="1">
         <v>99</v>
       </c>
@@ -34203,6 +34283,10 @@
       <c r="H16" s="69" t="s">
         <v>1</v>
       </c>
+      <c r="I16" s="1">
+        <f>SUM($F16:F$93)</f>
+        <v>156</v>
+      </c>
       <c r="L16" s="1">
         <v>102</v>
       </c>
@@ -34241,6 +34325,10 @@
       <c r="H17" s="69" t="s">
         <v>99</v>
       </c>
+      <c r="I17" s="1">
+        <f>SUM($F17:F$93)</f>
+        <v>150</v>
+      </c>
       <c r="L17" s="1">
         <v>103</v>
       </c>
@@ -34279,6 +34367,10 @@
       <c r="H18" s="69" t="s">
         <v>5</v>
       </c>
+      <c r="I18" s="1">
+        <f>SUM($F18:F$93)</f>
+        <v>144</v>
+      </c>
       <c r="L18" s="1">
         <v>107</v>
       </c>
@@ -34317,6 +34409,10 @@
       <c r="H19" s="69" t="s">
         <v>24</v>
       </c>
+      <c r="I19" s="1">
+        <f>SUM($F19:F$93)</f>
+        <v>138</v>
+      </c>
       <c r="L19" s="1">
         <v>110</v>
       </c>
@@ -34355,6 +34451,10 @@
       <c r="H20" s="69" t="s">
         <v>32</v>
       </c>
+      <c r="I20" s="1">
+        <f>SUM($F20:F$93)</f>
+        <v>128</v>
+      </c>
       <c r="L20" s="1">
         <v>111</v>
       </c>
@@ -34393,6 +34493,10 @@
       <c r="H21" s="69" t="s">
         <v>123</v>
       </c>
+      <c r="I21" s="1">
+        <f>SUM($F21:F$93)</f>
+        <v>122</v>
+      </c>
       <c r="L21" s="1">
         <v>112</v>
       </c>
@@ -34431,6 +34535,10 @@
       <c r="H22" s="69" t="s">
         <v>87</v>
       </c>
+      <c r="I22" s="1">
+        <f>SUM($F22:F$93)</f>
+        <v>119</v>
+      </c>
       <c r="L22" s="1">
         <v>113</v>
       </c>
@@ -34469,6 +34577,10 @@
       <c r="H23" s="69" t="s">
         <v>87</v>
       </c>
+      <c r="I23" s="1">
+        <f>SUM($F23:F$93)</f>
+        <v>116</v>
+      </c>
       <c r="L23" s="1">
         <v>114</v>
       </c>
@@ -34507,6 +34619,10 @@
       <c r="H24" s="69" t="s">
         <v>14</v>
       </c>
+      <c r="I24" s="1">
+        <f>SUM($F24:F$93)</f>
+        <v>113</v>
+      </c>
       <c r="L24" s="1">
         <v>114</v>
       </c>
@@ -34545,6 +34661,10 @@
       <c r="H25" s="69" t="s">
         <v>53</v>
       </c>
+      <c r="I25" s="1">
+        <f>SUM($F25:F$93)</f>
+        <v>112</v>
+      </c>
       <c r="L25" s="1">
         <v>114</v>
       </c>
@@ -34583,6 +34703,10 @@
       <c r="H26" s="69" t="s">
         <v>72</v>
       </c>
+      <c r="I26" s="1">
+        <f>SUM($F26:F$93)</f>
+        <v>106</v>
+      </c>
       <c r="L26" s="1">
         <v>117</v>
       </c>
@@ -34621,7 +34745,10 @@
       <c r="H27" s="69" t="s">
         <v>78</v>
       </c>
-      <c r="I27" s="69"/>
+      <c r="I27" s="1">
+        <f>SUM($F27:F$93)</f>
+        <v>100</v>
+      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
@@ -34646,7 +34773,10 @@
       <c r="H28" s="69" t="s">
         <v>141</v>
       </c>
-      <c r="I28" s="69"/>
+      <c r="I28" s="1">
+        <f>SUM($F28:F$93)</f>
+        <v>97</v>
+      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
@@ -34673,6 +34803,10 @@
       <c r="H29" s="69" t="s">
         <v>201</v>
       </c>
+      <c r="I29" s="1">
+        <f>SUM($F29:F$93)</f>
+        <v>97</v>
+      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
@@ -34699,6 +34833,10 @@
       <c r="H30" s="69" t="s">
         <v>63</v>
       </c>
+      <c r="I30" s="1">
+        <f>SUM($F30:F$93)</f>
+        <v>96</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
@@ -34725,6 +34863,10 @@
       <c r="H31" s="69" t="s">
         <v>97</v>
       </c>
+      <c r="I31" s="1">
+        <f>SUM($F31:F$93)</f>
+        <v>90</v>
+      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
@@ -34751,8 +34893,12 @@
       <c r="H32" s="69" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="1">
+        <f>SUM($F32:F$93)</f>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
         <v>126</v>
       </c>
@@ -34777,8 +34923,12 @@
       <c r="H33" s="69" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="1">
+        <f>SUM($F33:F$93)</f>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
         <v>81</v>
       </c>
@@ -34803,8 +34953,12 @@
       <c r="H34" s="69" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I34" s="1">
+        <f>SUM($F34:F$93)</f>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
         <v>133</v>
       </c>
@@ -34829,8 +34983,12 @@
       <c r="H35" s="69" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I35" s="1">
+        <f>SUM($F35:F$93)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
         <v>124</v>
       </c>
@@ -34855,8 +35013,12 @@
       <c r="H36" s="69" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I36" s="1">
+        <f>SUM($F36:F$93)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
         <v>256</v>
       </c>
@@ -34881,8 +35043,12 @@
       <c r="H37" s="69" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I37" s="1">
+        <f>SUM($F37:F$93)</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="35" t="s">
         <v>149</v>
       </c>
@@ -34905,8 +35071,12 @@
       <c r="H38" s="69" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I38" s="1">
+        <f>SUM($F38:F$93)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="35" t="s">
         <v>105</v>
       </c>
@@ -34931,8 +35101,12 @@
       <c r="H39" s="69" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I39" s="1">
+        <f>SUM($F39:F$93)</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>209</v>
       </c>
@@ -34957,8 +35131,12 @@
       <c r="H40" s="69" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I40" s="1">
+        <f>SUM($F40:F$93)</f>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>135</v>
       </c>
@@ -34983,8 +35161,12 @@
       <c r="H41" s="69" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I41" s="1">
+        <f>SUM($F41:F$93)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
         <v>177</v>
       </c>
@@ -35009,8 +35191,12 @@
       <c r="H42" s="69" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I42" s="1">
+        <f>SUM($F42:F$93)</f>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
         <v>269</v>
       </c>
@@ -35033,8 +35219,12 @@
       <c r="H43" s="69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I43" s="1">
+        <f>SUM($F43:F$93)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
         <v>337</v>
       </c>
@@ -35059,8 +35249,12 @@
       <c r="H44" s="69" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I44" s="1">
+        <f>SUM($F44:F$93)</f>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
         <v>60</v>
       </c>
@@ -35085,8 +35279,12 @@
       <c r="H45" s="69" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I45" s="1">
+        <f>SUM($F45:F$93)</f>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>146</v>
       </c>
@@ -35111,8 +35309,12 @@
       <c r="H46" s="69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I46" s="1">
+        <f>SUM($F46:F$93)</f>
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>143</v>
       </c>
@@ -35137,8 +35339,12 @@
       <c r="H47" s="69" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I47" s="1">
+        <f>SUM($F47:F$93)</f>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>150</v>
       </c>
@@ -35163,8 +35369,12 @@
       <c r="H48" s="69" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I48" s="1">
+        <f>SUM($F48:F$93)</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="35" t="s">
         <v>247</v>
       </c>
@@ -35189,8 +35399,12 @@
       <c r="H49" s="69" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I49" s="1">
+        <f>SUM($F49:F$93)</f>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="35" t="s">
         <v>166</v>
       </c>
@@ -35215,8 +35429,12 @@
       <c r="H50" s="69" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I50" s="1">
+        <f>SUM($F50:F$93)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
         <v>258</v>
       </c>
@@ -35241,8 +35459,12 @@
       <c r="H51" s="69" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I51" s="1">
+        <f>SUM($F51:F$93)</f>
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
         <v>93</v>
       </c>
@@ -35267,8 +35489,12 @@
       <c r="H52" s="69" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I52" s="1">
+        <f>SUM($F52:F$93)</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
         <v>228</v>
       </c>
@@ -35293,8 +35519,12 @@
       <c r="H53" s="69" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I53" s="1">
+        <f>SUM($F53:F$93)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
         <v>133</v>
       </c>
@@ -35319,8 +35549,12 @@
       <c r="H54" s="69" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I54" s="1">
+        <f>SUM($F54:F$93)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="35" t="s">
         <v>234</v>
       </c>
@@ -35345,8 +35579,12 @@
       <c r="H55" s="69" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I55" s="1">
+        <f>SUM($F55:F$93)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
         <v>290</v>
       </c>
@@ -35369,8 +35607,12 @@
       <c r="H56" s="69" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I56" s="1">
+        <f>SUM($F56:F$93)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="35" t="s">
         <v>137</v>
       </c>
@@ -35395,8 +35637,12 @@
       <c r="H57" s="69" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I57" s="1">
+        <f>SUM($F57:F$93)</f>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
         <v>113</v>
       </c>
@@ -35421,8 +35667,12 @@
       <c r="H58" s="69" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I58" s="1">
+        <f>SUM($F58:F$93)</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
         <v>183</v>
       </c>
@@ -35447,8 +35697,12 @@
       <c r="H59" s="69" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I59" s="1">
+        <f>SUM($F59:F$93)</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
         <v>103</v>
       </c>
@@ -35473,8 +35727,12 @@
       <c r="H60" s="69" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I60" s="1">
+        <f>SUM($F60:F$93)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="35" t="s">
         <v>191</v>
       </c>
@@ -35499,8 +35757,12 @@
       <c r="H61" s="69" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I61" s="1">
+        <f>SUM($F61:F$93)</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="35" t="s">
         <v>345</v>
       </c>
@@ -35525,8 +35787,12 @@
       <c r="H62" s="69" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I62" s="1">
+        <f>SUM($F62:F$93)</f>
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="35" t="s">
         <v>130</v>
       </c>
@@ -35551,8 +35817,12 @@
       <c r="H63" s="69" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I63" s="1">
+        <f>SUM($F63:F$93)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="35" t="s">
         <v>159</v>
       </c>
@@ -35577,8 +35847,12 @@
       <c r="H64" s="69" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I64" s="1">
+        <f>SUM($F64:F$93)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="35" t="s">
         <v>236</v>
       </c>
@@ -35603,8 +35877,12 @@
       <c r="H65" s="69" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I65" s="1">
+        <f>SUM($F65:F$93)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
         <v>172</v>
       </c>
@@ -35629,8 +35907,12 @@
       <c r="H66" s="69" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I66" s="1">
+        <f>SUM($F66:F$93)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="35" t="s">
         <v>186</v>
       </c>
@@ -35655,8 +35937,12 @@
       <c r="H67" s="69" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I67" s="1">
+        <f>SUM($F67:F$93)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="35" t="s">
         <v>285</v>
       </c>
@@ -35681,8 +35967,12 @@
       <c r="H68" s="69" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I68" s="1">
+        <f>SUM($F68:F$93)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="35" t="s">
         <v>180</v>
       </c>
@@ -35707,8 +35997,12 @@
       <c r="H69" s="69" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I69" s="1">
+        <f>SUM($F69:F$93)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="35" t="s">
         <v>362</v>
       </c>
@@ -35731,8 +36025,12 @@
       <c r="H70" s="69" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I70" s="1">
+        <f>SUM($F70:F$93)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="35" t="s">
         <v>152</v>
       </c>
@@ -35757,8 +36055,12 @@
       <c r="H71" s="69" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I71" s="1">
+        <f>SUM($F71:F$93)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="35" t="s">
         <v>265</v>
       </c>
@@ -35783,8 +36085,12 @@
       <c r="H72" s="69" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I72" s="1">
+        <f>SUM($F72:F$93)</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="35" t="s">
         <v>182</v>
       </c>
@@ -35809,8 +36115,12 @@
       <c r="H73" s="69" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I73" s="1">
+        <f>SUM($F73:F$93)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="35" t="s">
         <v>226</v>
       </c>
@@ -35835,8 +36145,12 @@
       <c r="H74" s="69" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I74" s="1">
+        <f>SUM($F74:F$93)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="35" t="s">
         <v>158</v>
       </c>
@@ -35861,8 +36175,12 @@
       <c r="H75" s="69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I75" s="1">
+        <f>SUM($F75:F$93)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="35" t="s">
         <v>252</v>
       </c>
@@ -35887,8 +36205,12 @@
       <c r="H76" s="69" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I76" s="1">
+        <f>SUM($F76:F$93)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="35" t="s">
         <v>216</v>
       </c>
@@ -35911,8 +36233,12 @@
       <c r="H77" s="69" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I77" s="1">
+        <f>SUM($F77:F$93)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="35" t="s">
         <v>492</v>
       </c>
@@ -35935,8 +36261,12 @@
       <c r="H78" s="69" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I78" s="1">
+        <f>SUM($F78:F$93)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="35" t="s">
         <v>229</v>
       </c>
@@ -35959,8 +36289,12 @@
       <c r="H79" s="69" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I79" s="1">
+        <f>SUM($F79:F$93)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="35" t="s">
         <v>793</v>
       </c>
@@ -35983,8 +36317,12 @@
       <c r="H80" s="69" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I80" s="1">
+        <f>SUM($F80:F$93)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="35" t="s">
         <v>369</v>
       </c>
@@ -36007,8 +36345,12 @@
       <c r="H81" s="69" t="s">
         <v>1098</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I81" s="1">
+        <f>SUM($F81:F$93)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="35" t="s">
         <v>230</v>
       </c>
@@ -36033,8 +36375,12 @@
       <c r="H82" s="69" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I82" s="1">
+        <f>SUM($F82:F$93)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="35" t="s">
         <v>155</v>
       </c>
@@ -36059,8 +36405,12 @@
       <c r="H83" s="69" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I83" s="1">
+        <f>SUM($F83:F$93)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="35" t="s">
         <v>195</v>
       </c>
@@ -36085,8 +36435,12 @@
       <c r="H84" s="69" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I84" s="1">
+        <f>SUM($F84:F$93)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="35" t="s">
         <v>188</v>
       </c>
@@ -36111,8 +36465,12 @@
       <c r="H85" s="69" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I85" s="1">
+        <f>SUM($F85:F$93)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="71" t="s">
         <v>502</v>
       </c>
@@ -36137,8 +36495,12 @@
       <c r="H86" s="73" t="s">
         <v>503</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I86" s="1">
+        <f>SUM($F86:F$93)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="35" t="s">
         <v>231</v>
       </c>
@@ -36163,8 +36525,12 @@
       <c r="H87" s="69" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I87" s="1">
+        <f>SUM($F87:F$93)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="35" t="s">
         <v>429</v>
       </c>
@@ -36187,8 +36553,12 @@
       <c r="H88" s="69" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I88" s="1">
+        <f>SUM($F88:F$93)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="35" t="s">
         <v>449</v>
       </c>
@@ -36211,8 +36581,12 @@
       <c r="H89" s="69" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I89" s="1">
+        <f>SUM($F89:F$93)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="35" t="s">
         <v>483</v>
       </c>
@@ -36235,8 +36609,12 @@
       <c r="H90" s="69" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I90" s="1">
+        <f>SUM($F90:F$93)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="35" t="s">
         <v>196</v>
       </c>
@@ -36259,8 +36637,12 @@
       <c r="H91" s="69" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I91" s="1">
+        <f>SUM($F91:F$93)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="35" t="s">
         <v>219</v>
       </c>
@@ -36285,8 +36667,12 @@
       <c r="H92" s="69" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I92" s="1">
+        <f>SUM($F92:F$93)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="35" t="s">
         <v>322</v>
       </c>
@@ -36311,20 +36697,24 @@
       <c r="H93" s="69" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I93">
+        <f>SUM($F$93:F93)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="8"/>
       <c r="C94" s="21"/>
       <c r="D94" s="1"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="8"/>
       <c r="B95" s="8"/>
       <c r="C95" s="21"/>
       <c r="D95" s="1"/>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="8"/>
       <c r="C96" s="21"/>

</xml_diff>